<commit_message>
now we can handle trade, repo, fx in one call to python main.py
</commit_message>
<xml_diff>
--- a/samples/sample_fx.xlsx
+++ b/samples/sample_fx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.zhang\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\boci_trustee\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E610B0E-18BD-42DD-BE72-189C81CAA07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB4422A-8A4C-4AA6-9280-4F07AA7576B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="750" windowWidth="17445" windowHeight="14565"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t5213805" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="27">
   <si>
     <t>China Life Franklin</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>HKD</t>
-  </si>
-  <si>
-    <t>SOCIETE GENERALE</t>
-  </si>
-  <si>
-    <t>NOMURA HOLDINGS</t>
   </si>
   <si>
     <t>USD/HKD R 12/28/20</t>
@@ -112,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -947,24 +941,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="8" max="8" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -996,7 +997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1092,7 +1093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1124,76 +1125,82 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>296334</v>
+        <v>296304</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8">
-        <v>200000</v>
+        <v>1500</v>
       </c>
       <c r="I8">
-        <v>105.971</v>
+        <v>7.7521000000000004</v>
       </c>
       <c r="J8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9">
-        <v>296336</v>
+        <v>296306</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H9">
-        <v>200000</v>
+        <v>23000</v>
       </c>
       <c r="I9">
-        <v>104.977</v>
+        <v>7.7470999999999997</v>
       </c>
       <c r="J9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
-        <v>296304</v>
+        <v>296308</v>
       </c>
       <c r="C10" t="s">
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
@@ -1205,108 +1212,44 @@
         <v>16</v>
       </c>
       <c r="H10">
-        <v>1500</v>
+        <v>18000</v>
       </c>
       <c r="I10">
-        <v>7.7521000000000004</v>
+        <v>7.7516999999999996</v>
       </c>
       <c r="J10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>296306</v>
+        <v>296316</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H11">
-        <v>23000</v>
+        <v>59344.402776000003</v>
       </c>
       <c r="I11">
-        <v>7.7470999999999997</v>
+        <v>0.84253999999999996</v>
       </c>
       <c r="J11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>296308</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12">
-        <v>18000</v>
-      </c>
-      <c r="I12">
-        <v>7.7516999999999996</v>
-      </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>296316</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13">
-        <v>59344.402776000003</v>
-      </c>
-      <c r="I13">
-        <v>0.84253999999999996</v>
-      </c>
-      <c r="J13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added fx trade conversion to the package
</commit_message>
<xml_diff>
--- a/samples/sample_fx.xlsx
+++ b/samples/sample_fx.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhangst\git\boci_trustee\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB4422A-8A4C-4AA6-9280-4F07AA7576B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE18018-0033-4295-8F2F-3C7E543B1246}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1308" yWindow="0" windowWidth="18264" windowHeight="12624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t5213805" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -945,7 +956,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1049,7 +1060,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="1">
-        <v>44198</v>
+        <v>44228</v>
       </c>
       <c r="H5">
         <v>50000</v>

</xml_diff>